<commit_message>
Adding info about cases that aren't good.
</commit_message>
<xml_diff>
--- a/BuffetWorkingGroup/TestCase1b/cuts-setup.xlsx
+++ b/BuffetWorkingGroup/TestCase1b/cuts-setup.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwpomero/crm/hs/dpw-8/github/DPW8-Plotting/BuffetWorkingGroup/TestCase1b/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99854342-CF42-D84E-B2DD-FC9C50F01945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17958A8-64DD-9F4E-8ABE-86EC035A33F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="19980" windowHeight="14580" xr2:uid="{EF8968BA-7CDB-2C41-AF7E-5BD1621428BB}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="27480" windowHeight="17160" xr2:uid="{EF8968BA-7CDB-2C41-AF7E-5BD1621428BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="136">
   <si>
     <t>002.01</t>
   </si>
@@ -284,6 +284,9 @@
     <t>SA-noft2</t>
   </si>
   <si>
+    <t>DDES</t>
+  </si>
+  <si>
     <t>SA-RC-comp-neg</t>
   </si>
   <si>
@@ -432,6 +435,18 @@
   </si>
   <si>
     <t>CP Zone End</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>021.03</t>
+  </si>
+  <si>
+    <t>021.04</t>
+  </si>
+  <si>
+    <t>Extruded Cadence Unstructured</t>
   </si>
 </sst>
 </file>
@@ -828,11 +843,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAFC31F-0382-344A-890D-6EB0F99DBB1B}">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -843,7 +858,7 @@
     <col min="5" max="5" width="15.6640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="33.5" style="4" customWidth="1"/>
     <col min="7" max="13" width="15" style="4" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -852,13 +867,13 @@
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>56</v>
@@ -867,25 +882,25 @@
         <v>57</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>58</v>
@@ -903,16 +918,16 @@
         <v>59</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>61</v>
@@ -923,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D58" si="0">CONCATENATE(B3,"-",C3)</f>
+        <f t="shared" ref="D3:D60" si="0">CONCATENATE(B3,"-",C3)</f>
         <v>-</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -951,10 +966,10 @@
         <v>59</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>61</v>
@@ -972,19 +987,19 @@
         <v>59</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -999,19 +1014,19 @@
         <v>59</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1047,13 +1062,13 @@
         <v>59</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>60</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>61</v>
@@ -1071,13 +1086,13 @@
         <v>59</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>60</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>61</v>
@@ -1101,7 +1116,7 @@
         <v>60</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1116,28 +1131,28 @@
         <v>59</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="4">
-        <f>C12</f>
-        <v>0</v>
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>72</v>
@@ -1149,16 +1164,16 @@
         <v>60</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4">
-        <f>C13</f>
-        <v>0</v>
+      <c r="D13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>72</v>
@@ -1170,31 +1185,31 @@
         <v>60</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4">
-        <f>C14</f>
-        <v>0</v>
+      <c r="D14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>60</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1209,13 +1224,13 @@
         <v>59</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>61</v>
@@ -1233,13 +1248,13 @@
         <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>61</v>
@@ -1254,13 +1269,13 @@
         <v>-</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>61</v>
@@ -1281,7 +1296,7 @@
         <v>74</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>61</v>
@@ -1305,10 +1320,10 @@
         <v>60</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1329,16 +1344,16 @@
         <v>60</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1353,16 +1368,16 @@
         <v>59</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1377,13 +1392,13 @@
         <v>59</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>77</v>
@@ -1401,19 +1416,19 @@
         <v>59</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>77</v>
@@ -1431,7 +1446,7 @@
         <v>59</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>60</v>
@@ -1458,7 +1473,7 @@
         <v>60</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>77</v>
@@ -1482,10 +1497,10 @@
         <v>60</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>77</v>
@@ -1509,13 +1524,13 @@
         <v>60</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>77</v>
@@ -1536,7 +1551,7 @@
         <v>67</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>77</v>
@@ -1575,13 +1590,13 @@
         <v>59</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>60</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>61</v>
@@ -1599,16 +1614,16 @@
         <v>59</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>60</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>61</v>
@@ -1647,13 +1662,13 @@
         <v>59</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>61</v>
@@ -1667,14 +1682,17 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
+      <c r="E34" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="F34" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>60</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>61</v>
@@ -1698,10 +1716,10 @@
         <v>60</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>61</v>
@@ -1719,16 +1737,16 @@
         <v>59</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>60</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>61</v>
@@ -1746,19 +1764,19 @@
         <v>59</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>61</v>
@@ -1782,13 +1800,13 @@
         <v>60</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>61</v>
@@ -1806,22 +1824,22 @@
         <v>59</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>61</v>
@@ -1842,16 +1860,16 @@
         <v>79</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1872,7 +1890,7 @@
         <v>60</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>61</v>
@@ -1896,7 +1914,7 @@
         <v>60</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>61</v>
@@ -1906,9 +1924,9 @@
       <c r="A43" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="4">
-        <f>C43</f>
-        <v>0</v>
+      <c r="D43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>62</v>
@@ -1959,7 +1977,7 @@
         <v>75</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>61</v>
@@ -1977,13 +1995,13 @@
         <v>59</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>60</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1998,13 +2016,13 @@
         <v>59</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>60</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2025,7 +2043,7 @@
         <v>60</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -2051,7 +2069,7 @@
     </row>
     <row r="50" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D50" s="4" t="str">
         <f>CONCATENATE(B50,"-",C50)</f>
@@ -2061,16 +2079,16 @@
         <v>59</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>61</v>
@@ -2078,7 +2096,7 @@
     </row>
     <row r="51" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D51" s="4" t="str">
         <f>CONCATENATE(B51,"-",C51)</f>
@@ -2088,16 +2106,16 @@
         <v>62</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>61</v>
@@ -2105,33 +2123,53 @@
     </row>
     <row r="52" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D52" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>133</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="J52" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="N52" s="4" t="s">
-        <v>61</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>127</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N53" s="4" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D54" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2141,7 +2179,7 @@
         <v>59</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>60</v>
@@ -2152,7 +2190,7 @@
     </row>
     <row r="55" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="D55" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2165,10 +2203,7 @@
         <v>60</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>61</v>
@@ -2176,7 +2211,7 @@
     </row>
     <row r="56" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D56" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2186,16 +2221,10 @@
         <v>59</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="M56" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>61</v>
@@ -2203,7 +2232,7 @@
     </row>
     <row r="57" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D57" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2213,18 +2242,21 @@
         <v>59</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>105</v>
+        <v>60</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D58" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2234,74 +2266,121 @@
         <v>59</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="H58" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="N58" s="4" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D59" s="4" t="str">
-        <f t="shared" ref="D59:D60" si="1">CONCATENATE(B59,"-",C59)</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D60" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="K60" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="N60" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
-        <v>128</v>
+        <v>53</v>
+      </c>
+      <c r="D61" s="4" t="str">
+        <f t="shared" ref="D61:D62" si="1">CONCATENATE(B61,"-",C61)</f>
+        <v>-</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N62" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N60" xr:uid="{EAAFC31F-0382-344A-890D-6EB0F99DBB1B}"/>
+  <autoFilter ref="A1:N62" xr:uid="{EAAFC31F-0382-344A-890D-6EB0F99DBB1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A63:C1048576 N63:XFD1048576 R54:XFD60 E34 A1 A54:A60 E63:F1048576 A31:A37 A30 A39:A42 A38 A2:A29 O1:XFD42 A43:A49 R44:XFD49 A50:A51 A52 R52:XFD52 D50:XFD51" numberStoredAsText="1"/>
-    <ignoredError sqref="D43" formula="1"/>
+    <ignoredError sqref="A65:C1048576 N65:XFD1048576 R56:XFD62 E65:F1048576 O1:XFD42 R44:XFD49 A54:A63 R54:XFD54 D50:XFD51 A1:A51 A52:A53" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All kinds of new work
</commit_message>
<xml_diff>
--- a/BuffetWorkingGroup/TestCase1b/cuts-setup.xlsx
+++ b/BuffetWorkingGroup/TestCase1b/cuts-setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwpomero/crm/hs/dpw-8/github/DPW8-Plotting/BuffetWorkingGroup/TestCase1b/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17958A8-64DD-9F4E-8ABE-86EC035A33F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAA23EF-7326-9745-8B81-E20C9011B8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="27480" windowHeight="17160" xr2:uid="{EF8968BA-7CDB-2C41-AF7E-5BD1621428BB}"/>
+    <workbookView xWindow="340" yWindow="1440" windowWidth="29160" windowHeight="18860" xr2:uid="{EF8968BA-7CDB-2C41-AF7E-5BD1621428BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="133">
   <si>
     <t>002.01</t>
   </si>
@@ -284,9 +284,6 @@
     <t>SA-noft2</t>
   </si>
   <si>
-    <t>DDES</t>
-  </si>
-  <si>
     <t>SA-RC-comp-neg</t>
   </si>
   <si>
@@ -419,9 +416,6 @@
     <t>021.01</t>
   </si>
   <si>
-    <t>021.02</t>
-  </si>
-  <si>
     <t>SA RC QCR</t>
   </si>
   <si>
@@ -437,16 +431,13 @@
     <t>CP Zone End</t>
   </si>
   <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>021.03</t>
-  </si>
-  <si>
-    <t>021.04</t>
-  </si>
-  <si>
-    <t>Extruded Cadence Unstructured</t>
+    <t>10.02</t>
+  </si>
+  <si>
+    <t>10.03</t>
+  </si>
+  <si>
+    <t>Adaptive Euler</t>
   </si>
 </sst>
 </file>
@@ -843,11 +834,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAFC31F-0382-344A-890D-6EB0F99DBB1B}">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -867,13 +858,13 @@
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>56</v>
@@ -882,25 +873,25 @@
         <v>57</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>58</v>
@@ -910,24 +901,30 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>60</v>
+      </c>
       <c r="D2" s="4" t="str">
         <f>CONCATENATE(B2,"-",C2)</f>
-        <v>-</v>
+        <v>1-60</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>61</v>
@@ -937,9 +934,15 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="4">
+        <v>61</v>
+      </c>
+      <c r="C3" s="4">
+        <v>120</v>
+      </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D60" si="0">CONCATENATE(B3,"-",C3)</f>
-        <v>-</v>
+        <f t="shared" ref="D3:D65" si="0">CONCATENATE(B3,"-",C3)</f>
+        <v>61-120</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>59</v>
@@ -958,18 +961,24 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="4">
+        <v>121</v>
+      </c>
+      <c r="C4" s="4">
+        <v>180</v>
+      </c>
       <c r="D4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>121-180</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>61</v>
@@ -979,63 +988,81 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="4">
+        <v>181</v>
+      </c>
+      <c r="C5" s="4">
+        <v>240</v>
+      </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>181-240</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="4">
+        <v>241</v>
+      </c>
+      <c r="C6" s="4">
+        <v>300</v>
+      </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>241-300</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="4">
+        <v>301</v>
+      </c>
+      <c r="C7" s="4">
+        <v>360</v>
+      </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>301-360</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>59</v>
@@ -1054,21 +1081,28 @@
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="4">
+        <v>361</v>
+      </c>
+      <c r="C8" s="4">
+        <f>B9-1</f>
+        <v>420</v>
+      </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>361-420</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>60</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>61</v>
@@ -1078,21 +1112,28 @@
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="4">
+        <v>421</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" ref="C9:C62" si="1">B10-1</f>
+        <v>480</v>
+      </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>421-480</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>60</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>61</v>
@@ -1102,9 +1143,16 @@
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B10" s="4">
+        <v>481</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="1"/>
+        <v>540</v>
+      </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>481-540</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>59</v>
@@ -1116,43 +1164,57 @@
         <v>60</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B11" s="4">
+        <v>541</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>541-600</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="4">
+        <v>601</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="1"/>
+        <v>610</v>
+      </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>601-610</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>72</v>
@@ -1164,16 +1226,23 @@
         <v>60</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="B13" s="4">
+        <v>611</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="1"/>
+        <v>620</v>
+      </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>611-620</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>72</v>
@@ -1185,52 +1254,66 @@
         <v>60</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B14" s="4">
+        <v>621</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="1"/>
+        <v>630</v>
+      </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>621-630</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>60</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B15" s="4">
+        <v>631</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="1"/>
+        <v>690</v>
+      </c>
       <c r="D15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>631-690</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>61</v>
@@ -1240,21 +1323,28 @@
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B16" s="4">
+        <v>691</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
       <c r="D16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>691-750</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>61</v>
@@ -1264,18 +1354,25 @@
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="B17" s="4">
+        <v>751</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="1"/>
+        <v>810</v>
+      </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>751-810</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>61</v>
@@ -1285,9 +1382,16 @@
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B18" s="4">
+        <v>811</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
       <c r="D18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>811-870</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>73</v>
@@ -1296,7 +1400,7 @@
         <v>74</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>61</v>
@@ -1306,9 +1410,16 @@
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B19" s="4">
+        <v>871</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="1"/>
+        <v>876</v>
+      </c>
       <c r="D19" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>CONCATENATE(B53,"-",C19)</f>
+        <v>2236-876</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>59</v>
@@ -1320,19 +1431,26 @@
         <v>60</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="B20" s="4">
+        <v>877</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="1"/>
+        <v>882</v>
+      </c>
       <c r="D20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>CONCATENATE(B54,"-",C20)</f>
+        <v>2296-882</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>59</v>
@@ -1344,61 +1462,75 @@
         <v>60</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B21" s="4">
+        <v>883</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="1"/>
+        <v>888</v>
+      </c>
       <c r="D21" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>CONCATENATE(B55,"-",C21)</f>
+        <v>2356-888</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B22" s="4">
+        <v>889</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="1"/>
+        <v>920</v>
+      </c>
       <c r="D22" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>CONCATENATE(B56,"-",C22)</f>
+        <v>2416-920</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>77</v>
@@ -1408,27 +1540,34 @@
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="B23" s="4">
+        <v>921</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" si="1"/>
+        <v>952</v>
+      </c>
       <c r="D23" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>CONCATENATE(B57,"-",C23)</f>
+        <v>2476-952</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>77</v>
@@ -1438,15 +1577,22 @@
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B24" s="4">
+        <v>953</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="1"/>
+        <v>984</v>
+      </c>
       <c r="D24" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>CONCATENATE(B58,"-",C24)</f>
+        <v>2536-984</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>60</v>
@@ -1459,9 +1605,16 @@
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B25" s="4">
+        <v>985</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="1"/>
+        <v>1006</v>
+      </c>
       <c r="D25" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <f>CONCATENATE(B59,"-",C25)</f>
+        <v>2551-1006</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>62</v>
@@ -1473,7 +1626,7 @@
         <v>60</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>77</v>
@@ -1483,9 +1636,16 @@
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B26" s="4">
+        <v>1007</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="1"/>
+        <v>1028</v>
+      </c>
       <c r="D26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1007-1028</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>62</v>
@@ -1497,10 +1657,10 @@
         <v>60</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>77</v>
@@ -1510,9 +1670,16 @@
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B27" s="4">
+        <v>1029</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="1"/>
+        <v>1050</v>
+      </c>
       <c r="D27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1029-1050</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>62</v>
@@ -1524,13 +1691,13 @@
         <v>60</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>77</v>
@@ -1540,9 +1707,16 @@
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B28" s="4">
+        <v>1051</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="1"/>
+        <v>1060</v>
+      </c>
       <c r="D28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1051-1060</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>66</v>
@@ -1551,7 +1725,7 @@
         <v>67</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>77</v>
@@ -1559,71 +1733,83 @@
     </row>
     <row r="29" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
-        <v>27</v>
+        <v>130</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1061</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="1"/>
+        <v>1070</v>
       </c>
       <c r="D29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1061-1070</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>28</v>
+        <v>131</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1071</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="1"/>
+        <v>1080</v>
       </c>
       <c r="D30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1071-1080</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1081</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="1"/>
+        <v>1140</v>
       </c>
       <c r="D31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1081-1140</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>61</v>
@@ -1631,20 +1817,30 @@
     </row>
     <row r="32" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1141</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="1"/>
+        <v>1200</v>
       </c>
       <c r="D32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1141-1200</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>60</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>61</v>
@@ -1652,23 +1848,33 @@
     </row>
     <row r="33" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1201</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="1"/>
+        <v>1260</v>
       </c>
       <c r="D33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1201-1260</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>120</v>
+      <c r="K33" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>61</v>
@@ -1676,23 +1882,27 @@
     </row>
     <row r="34" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1261</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="1"/>
+        <v>1320</v>
       </c>
       <c r="D34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1261-1320</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>61</v>
@@ -1700,26 +1910,30 @@
     </row>
     <row r="35" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1321</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="1"/>
+        <v>1380</v>
       </c>
       <c r="D35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1321-1380</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>61</v>
@@ -1727,11 +1941,18 @@
     </row>
     <row r="36" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1381</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="1"/>
+        <v>1440</v>
       </c>
       <c r="D36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1381-1440</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>59</v>
@@ -1743,10 +1964,7 @@
         <v>60</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>61</v>
@@ -1754,29 +1972,33 @@
     </row>
     <row r="37" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1441</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="1"/>
+        <v>1500</v>
       </c>
       <c r="D37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1441-1500</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>61</v>
@@ -1784,29 +2006,33 @@
     </row>
     <row r="38" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1501</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="1"/>
+        <v>1560</v>
       </c>
       <c r="D38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1501-1560</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J38" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="K38" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>61</v>
@@ -1814,32 +2040,36 @@
     </row>
     <row r="39" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1561</v>
+      </c>
+      <c r="C39" s="4">
+        <f t="shared" si="1"/>
+        <v>1620</v>
       </c>
       <c r="D39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1561-1620</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>61</v>
@@ -1847,50 +2077,76 @@
     </row>
     <row r="40" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1621</v>
+      </c>
+      <c r="C40" s="4">
+        <f t="shared" si="1"/>
+        <v>1680</v>
       </c>
       <c r="D40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1621-1680</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>106</v>
+        <v>60</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1681</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" si="1"/>
+        <v>1740</v>
       </c>
       <c r="D41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1681-1740</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>61</v>
@@ -1898,38 +2154,55 @@
     </row>
     <row r="42" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1741</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="1"/>
+        <v>1843</v>
       </c>
       <c r="D42" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1741-1843</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>122</v>
+        <v>105</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
-        <v>70</v>
+        <v>39</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1844</v>
+      </c>
+      <c r="C43" s="4">
+        <f t="shared" si="1"/>
+        <v>1863</v>
       </c>
       <c r="D43" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1844-1863</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>71</v>
@@ -1937,26 +2210,39 @@
       <c r="G43" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="H43" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="N43" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1864</v>
+      </c>
+      <c r="C44" s="4">
+        <f t="shared" si="1"/>
+        <v>1883</v>
       </c>
       <c r="D44" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1864-1883</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>60</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>61</v>
@@ -1964,20 +2250,27 @@
     </row>
     <row r="45" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
-        <v>42</v>
+        <v>70</v>
+      </c>
+      <c r="B45" s="4">
+        <v>1884</v>
+      </c>
+      <c r="C45" s="4">
+        <f t="shared" si="1"/>
+        <v>1886</v>
       </c>
       <c r="D45" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1884-1886</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>61</v>
@@ -1985,137 +2278,167 @@
     </row>
     <row r="46" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1887</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" si="1"/>
+        <v>1936</v>
       </c>
       <c r="D46" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1887-1936</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>60</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1937</v>
+      </c>
+      <c r="C47" s="4">
+        <f t="shared" si="1"/>
+        <v>1986</v>
       </c>
       <c r="D47" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1937-1986</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1987</v>
+      </c>
+      <c r="C48" s="4">
+        <f t="shared" si="1"/>
+        <v>2046</v>
       </c>
       <c r="D48" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1987-2046</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>60</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B49" s="4">
+        <v>2047</v>
+      </c>
+      <c r="C49" s="4">
+        <f t="shared" si="1"/>
+        <v>2055</v>
       </c>
       <c r="D49" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2047-2055</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>60</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
-        <v>125</v>
+        <v>45</v>
+      </c>
+      <c r="B50" s="4">
+        <v>2056</v>
+      </c>
+      <c r="C50" s="4">
+        <f t="shared" si="1"/>
+        <v>2115</v>
       </c>
       <c r="D50" s="4" t="str">
-        <f>CONCATENATE(B50,"-",C50)</f>
-        <v>-</v>
+        <f t="shared" si="0"/>
+        <v>2056-2115</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J50" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="N50" s="4" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
-        <v>126</v>
+        <v>46</v>
+      </c>
+      <c r="B51" s="4">
+        <v>2116</v>
+      </c>
+      <c r="C51" s="4">
+        <f t="shared" si="1"/>
+        <v>2175</v>
       </c>
       <c r="D51" s="4" t="str">
-        <f>CONCATENATE(B51,"-",C51)</f>
-        <v>-</v>
+        <f t="shared" si="0"/>
+        <v>2116-2175</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>61</v>
@@ -2123,57 +2446,80 @@
     </row>
     <row r="52" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
+      </c>
+      <c r="B52" s="4">
+        <v>2176</v>
+      </c>
+      <c r="C52" s="4">
+        <f t="shared" si="1"/>
+        <v>2235</v>
+      </c>
+      <c r="D52" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>2176-2235</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>60</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
-        <v>134</v>
+        <v>47</v>
+      </c>
+      <c r="B53" s="4">
+        <v>2236</v>
+      </c>
+      <c r="C53" s="4">
+        <f t="shared" si="1"/>
+        <v>2295</v>
+      </c>
+      <c r="D53" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>2236-2295</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J53" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L53" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="N53" s="4" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
-        <v>47</v>
+        <v>126</v>
+      </c>
+      <c r="B54" s="4">
+        <v>2296</v>
+      </c>
+      <c r="C54" s="4">
+        <f t="shared" si="1"/>
+        <v>2355</v>
       </c>
       <c r="D54" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2296-2355</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>59</v>
@@ -2190,20 +2536,27 @@
     </row>
     <row r="55" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
-        <v>128</v>
+        <v>48</v>
+      </c>
+      <c r="B55" s="4">
+        <v>2356</v>
+      </c>
+      <c r="C55" s="4">
+        <f t="shared" si="1"/>
+        <v>2415</v>
       </c>
       <c r="D55" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2356-2415</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>61</v>
@@ -2211,20 +2564,30 @@
     </row>
     <row r="56" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="B56" s="4">
+        <v>2416</v>
+      </c>
+      <c r="C56" s="4">
+        <f t="shared" si="1"/>
+        <v>2475</v>
       </c>
       <c r="D56" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2416-2475</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>60</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>61</v>
@@ -2232,23 +2595,33 @@
     </row>
     <row r="57" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="B57" s="4">
+        <v>2476</v>
+      </c>
+      <c r="C57" s="4">
+        <f t="shared" si="1"/>
+        <v>2535</v>
       </c>
       <c r="D57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2476-2535</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>60</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>123</v>
+        <v>109</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>61</v>
@@ -2256,131 +2629,141 @@
     </row>
     <row r="58" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="B58" s="4">
+        <v>2536</v>
+      </c>
+      <c r="C58" s="4">
+        <f t="shared" si="1"/>
+        <v>2550</v>
       </c>
       <c r="D58" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2536-2550</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M58" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="B59" s="4">
+        <v>2551</v>
+      </c>
+      <c r="C59" s="4">
+        <f t="shared" si="1"/>
+        <v>2570</v>
       </c>
       <c r="D59" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2551-2570</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B60" s="4">
+        <v>2571</v>
+      </c>
+      <c r="C60" s="4">
+        <f t="shared" si="1"/>
+        <v>2588</v>
       </c>
       <c r="D60" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>2571-2588</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>60</v>
+        <v>105</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="B61" s="4">
+        <v>2589</v>
+      </c>
+      <c r="C61" s="4">
+        <f t="shared" si="1"/>
+        <v>2594</v>
       </c>
       <c r="D61" s="4" t="str">
-        <f t="shared" ref="D61:D62" si="1">CONCATENATE(B61,"-",C61)</f>
-        <v>-</v>
+        <f t="shared" si="0"/>
+        <v>2589-2594</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D62" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>127</v>
+      </c>
+      <c r="B62" s="4">
+        <v>2595</v>
+      </c>
+      <c r="D62" s="4">
+        <v>2595</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N62" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N62" xr:uid="{EAAFC31F-0382-344A-890D-6EB0F99DBB1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A65:C1048576 N65:XFD1048576 R56:XFD62 E65:F1048576 O1:XFD42 R44:XFD49 A54:A63 R54:XFD54 D50:XFD51 A1:A51 A52:A53" numberStoredAsText="1"/>
+    <ignoredError sqref="A85:C1048576 N64:XFD1048576 R55:XFD61 E64:F1048576 O31:XFD44 R46:XFD51 R53:XFD53 E52:XFD52 A31:A62 A64:A76 C64:C76 A1:A30 O1:XFD28 A77:A84 C77:C84" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>